<commit_message>
Rules 1.0 - 17/01/2026
</commit_message>
<xml_diff>
--- a/project-logs.xlsx
+++ b/project-logs.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abdurrahman Qureshi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\house-of-cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBA66AD5-3F7D-4B30-A1AF-35801F2AE5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38A4590C-32D8-4DB7-B861-A973184A5A6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>work</t>
   </si>
@@ -46,6 +46,12 @@
   </si>
   <si>
     <t>cards 2.0</t>
+  </si>
+  <si>
+    <t>UI Start</t>
+  </si>
+  <si>
+    <t>rules 0.5</t>
   </si>
 </sst>
 </file>
@@ -364,7 +370,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:D7"/>
+  <dimension ref="B2:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
@@ -416,6 +422,22 @@
         <v>5</v>
       </c>
     </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B8" s="1">
+        <v>46038</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B9" s="1">
+        <v>46039</v>
+      </c>
+      <c r="D9" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>